<commit_message>
made Team as String
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/template_8.xlsx
+++ b/src/main/resources/templates/template_8.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavelkozlov/Documents/bracket_excel/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavelkozlov/IdeaProjects/brackets-excel/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5336090E-D12A-C34A-BF0C-444313FF28A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E23E01-C51B-9649-8926-BFACB341B144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{D19B6972-C7AC-C346-9C8E-973E54F06BB3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20100" xr2:uid="{D19B6972-C7AC-C346-9C8E-973E54F06BB3}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8101A3AA-9363-1948-9E02-0BD3DC295EC8}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{8101A3AA-9363-1948-9E02-0BD3DC295EC8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    jx:area(lastCell="P46")</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Возр   кат.</t>
   </si>
@@ -60,13 +78,58 @@
   </si>
   <si>
     <t>Секретарь</t>
+  </si>
+  <si>
+    <t>${tournamentName}</t>
+  </si>
+  <si>
+    <t>${birthYearRange}</t>
+  </si>
+  <si>
+    <t>${weightCategory}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(7).participant.lastName} ${graph.get("THREE").get(7).participant.firstName} ${graph.get("THREE").get(7).participant.team? "(" + graph.get("THREE").get(7).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(6).participant.lastName} ${graph.get("THREE").get(6).participant.firstName} ${graph.get("THREE").get(6).participant.team? "(" + graph.get("THREE").get(6).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(5).participant.lastName} ${graph.get("THREE").get(5).participant.firstName} ${graph.get("THREE").get(5).participant.team? "(" + graph.get("THREE").get(5).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(4).participant.lastName} ${graph.get("THREE").get(4).participant.firstName} ${graph.get("THREE").get(4).participant.team? "(" + graph.get("THREE").get(4).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(3).participant.lastName} ${graph.get("THREE").get(3).participant.firstName} ${graph.get("THREE").get(3).participant.team? "(" + graph.get("THREE").get(3).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(2).participant.lastName} ${graph.get("THREE").get(2).participant.firstName} ${graph.get("THREE").get(2).participant.team? "(" + graph.get("THREE").get(2).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(1).participant.lastName} ${graph.get("THREE").get(1).participant.firstName} ${graph.get("THREE").get(1).participant.team? "(" + graph.get("THREE").get(1).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("THREE").get(0).participant.lastName} ${graph.get("THREE").get(0).participant.firstName} ${graph.get("THREE").get(0).participant.team? "(" + graph.get("THREE").get(0).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("TWO").get(0).participant.lastName} ${graph.get("TWO").get(0).participant.firstName} ${graph.get("TWO").get(0).participant.team? "(" + graph.get("TWO").get(0).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("TWO").get(1).participant.lastName} ${graph.get("TWO").get(1).participant.firstName} ${graph.get("TWO").get(1).participant.team? "(" + graph.get("TWO").get(1).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("TWO").get(2).participant.lastName} ${graph.get("TWO").get(2).participant.firstName} ${graph.get("TWO").get(2).participant.team? "(" + graph.get("TWO").get(2).participant.team + ")" : null}</t>
+  </si>
+  <si>
+    <t>${graph.get("TWO").get(3).participant.lastName} ${graph.get("TWO").get(3).participant.firstName} ${graph.get("TWO").get(3).participant.team? "(" + graph.get("TWO").get(3).participant.team + ")" : null}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,6 +152,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -154,13 +224,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -185,6 +258,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="13" id="{89C9EEC3-BD86-9E4D-8206-313CF2807FEA}" userId="S::13@mhwu.onmicrosoft.com::9a2a7ed0-a5ee-47c6-a916-7416c7a461e6" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,12 +561,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2023-12-30T20:56:58.63" personId="{89C9EEC3-BD86-9E4D-8206-313CF2807FEA}" id="{8101A3AA-9363-1948-9E02-0BD3DC295EC8}">
+    <text>jx:area(lastCell="P46")</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456BD6FC-31AD-864B-9636-CCD955A5DDDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456BD6FC-31AD-864B-9636-CCD955A5DDDB}">
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,53 +582,57 @@
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="C1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="1"/>
       <c r="N3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -577,7 +668,9 @@
       <c r="N5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
@@ -669,7 +762,9 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
@@ -688,7 +783,9 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
@@ -703,7 +800,9 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4"/>
       <c r="E14" s="1"/>
@@ -737,7 +836,9 @@
       <c r="A16" s="1">
         <v>3</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
@@ -756,7 +857,9 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
@@ -771,7 +874,9 @@
       <c r="A18" s="1">
         <v>4</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4"/>
       <c r="E18" s="1"/>
@@ -837,7 +942,9 @@
       <c r="A22" s="1">
         <v>5</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -856,7 +963,9 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="1"/>
@@ -871,7 +980,9 @@
       <c r="A24" s="1">
         <v>6</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="4"/>
       <c r="E24" s="1"/>
@@ -905,7 +1016,9 @@
       <c r="A26" s="1">
         <v>7</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
@@ -924,7 +1037,9 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="4"/>
       <c r="H27" s="1"/>
@@ -939,7 +1054,9 @@
       <c r="A28" s="1">
         <v>8</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4"/>
       <c r="E28" s="1"/>
@@ -973,10 +1090,10 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="6"/>
+      <c r="L32" s="7"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
@@ -1198,5 +1315,6 @@
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>